<commit_message>
fix: discard number if he smaller than previous number
</commit_message>
<xml_diff>
--- a/Resources/finaldata.xlsx
+++ b/Resources/finaldata.xlsx
@@ -869,13 +869,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:EO167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:145">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -900,194 +900,1232 @@
       <c r="I1" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="1">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="1">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="1">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="1">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="1">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="1">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="1">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="1">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="1">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="1">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="1">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="1">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="1">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="1">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="1">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="1">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="1">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="1">
+        <v>80</v>
+      </c>
+      <c r="CE1" s="1">
+        <v>81</v>
+      </c>
+      <c r="CF1" s="1">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="1">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="1">
+        <v>84</v>
+      </c>
+      <c r="CI1" s="1">
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="1">
+        <v>86</v>
+      </c>
+      <c r="CK1" s="1">
+        <v>87</v>
+      </c>
+      <c r="CL1" s="1">
+        <v>88</v>
+      </c>
+      <c r="CM1" s="1">
+        <v>89</v>
+      </c>
+      <c r="CN1" s="1">
+        <v>90</v>
+      </c>
+      <c r="CO1" s="1">
+        <v>91</v>
+      </c>
+      <c r="CP1" s="1">
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="1">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="1">
+        <v>94</v>
+      </c>
+      <c r="CS1" s="1">
+        <v>95</v>
+      </c>
+      <c r="CT1" s="1">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="1">
+        <v>97</v>
+      </c>
+      <c r="CV1" s="1">
+        <v>98</v>
+      </c>
+      <c r="CW1" s="1">
+        <v>99</v>
+      </c>
+      <c r="CX1" s="1">
+        <v>100</v>
+      </c>
+      <c r="CY1" s="1">
+        <v>101</v>
+      </c>
+      <c r="CZ1" s="1">
+        <v>102</v>
+      </c>
+      <c r="DA1" s="1">
+        <v>103</v>
+      </c>
+      <c r="DB1" s="1">
+        <v>104</v>
+      </c>
+      <c r="DC1" s="1">
+        <v>105</v>
+      </c>
+      <c r="DD1" s="1">
+        <v>106</v>
+      </c>
+      <c r="DE1" s="1">
+        <v>107</v>
+      </c>
+      <c r="DF1" s="1">
+        <v>108</v>
+      </c>
+      <c r="DG1" s="1">
+        <v>109</v>
+      </c>
+      <c r="DH1" s="1">
+        <v>110</v>
+      </c>
+      <c r="DI1" s="1">
+        <v>111</v>
+      </c>
+      <c r="DJ1" s="1">
+        <v>112</v>
+      </c>
+      <c r="DK1" s="1">
+        <v>113</v>
+      </c>
+      <c r="DL1" s="1">
+        <v>114</v>
+      </c>
+      <c r="DM1" s="1">
+        <v>115</v>
+      </c>
+      <c r="DN1" s="1">
+        <v>116</v>
+      </c>
+      <c r="DO1" s="1">
+        <v>117</v>
+      </c>
+      <c r="DP1" s="1">
+        <v>118</v>
+      </c>
+      <c r="DQ1" s="1">
+        <v>119</v>
+      </c>
+      <c r="DR1" s="1">
+        <v>120</v>
+      </c>
+      <c r="DS1" s="1">
+        <v>121</v>
+      </c>
+      <c r="DT1" s="1">
+        <v>122</v>
+      </c>
+      <c r="DU1" s="1">
+        <v>123</v>
+      </c>
+      <c r="DV1" s="1">
+        <v>124</v>
+      </c>
+      <c r="DW1" s="1">
+        <v>125</v>
+      </c>
+      <c r="DX1" s="1">
+        <v>126</v>
+      </c>
+      <c r="DY1" s="1">
+        <v>127</v>
+      </c>
+      <c r="DZ1" s="1">
+        <v>128</v>
+      </c>
+      <c r="EA1" s="1">
+        <v>129</v>
+      </c>
+      <c r="EB1" s="1">
+        <v>130</v>
+      </c>
+      <c r="EC1" s="1">
+        <v>131</v>
+      </c>
+      <c r="ED1" s="1">
+        <v>132</v>
+      </c>
+      <c r="EE1" s="1">
+        <v>133</v>
+      </c>
+      <c r="EF1" s="1">
+        <v>134</v>
+      </c>
+      <c r="EG1" s="1">
+        <v>135</v>
+      </c>
+      <c r="EH1" s="1">
+        <v>136</v>
+      </c>
+      <c r="EI1" s="1">
+        <v>137</v>
+      </c>
+      <c r="EJ1" s="1">
+        <v>138</v>
+      </c>
+      <c r="EK1" s="1">
+        <v>139</v>
+      </c>
+      <c r="EL1" s="1">
+        <v>140</v>
+      </c>
+      <c r="EM1" s="1">
+        <v>141</v>
+      </c>
+      <c r="EN1" s="1">
+        <v>142</v>
+      </c>
+      <c r="EO1" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:145">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="C2">
+        <v>66.6666666</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:145">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3">
+        <v>66.6666666</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="O3">
+        <v>33.3333333</v>
+      </c>
+      <c r="P3">
+        <v>133.3333332</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:145">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:145">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:145">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:145">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>33.3333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>933.3333324</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>2033.3333313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:145">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:145">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:145">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>33.3333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>599.9999994</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:145">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:145">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>233.3333331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>4766.6666619</v>
+      </c>
+    </row>
+    <row r="13" spans="1:145">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:145">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14">
-        <v>99.99999990000001</v>
+        <v>533.3333328</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:145">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="C15">
+        <v>99.99999990000001</v>
+      </c>
+      <c r="D15">
+        <v>33.3333333</v>
+      </c>
+      <c r="E15">
+        <v>33.3333333</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:145">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:54">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:54">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:54">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:54">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:54">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:54">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C22">
-        <v>33.3333333</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>366.6666663</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:54">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:54">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C24">
-        <v>66.6666666</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>866.6666658</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:54">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:54">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:54">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27">
-        <v>66.6666666</v>
+        <v>1166.6666655</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AQ27">
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <v>0</v>
+      </c>
+      <c r="AT27">
+        <v>0</v>
+      </c>
+      <c r="AU27">
+        <v>0</v>
+      </c>
+      <c r="AV27">
+        <v>0</v>
+      </c>
+      <c r="AW27">
+        <v>0</v>
+      </c>
+      <c r="AX27">
+        <v>0</v>
+      </c>
+      <c r="AY27">
+        <v>0</v>
+      </c>
+      <c r="AZ27">
+        <v>0</v>
+      </c>
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:54">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:54">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:54">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:54">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:54">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1172,22 +2210,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:69">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:69">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:69">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C51">
-        <v>233.3333331</v>
+        <v>4666.666662</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1198,236 +2236,689 @@
       <c r="F51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+      <c r="X51">
+        <v>0</v>
+      </c>
+      <c r="Y51">
+        <v>0</v>
+      </c>
+      <c r="Z51">
+        <v>0</v>
+      </c>
+      <c r="AA51">
+        <v>0</v>
+      </c>
+      <c r="AB51">
+        <v>0</v>
+      </c>
+      <c r="AC51">
+        <v>0</v>
+      </c>
+      <c r="AD51">
+        <v>0</v>
+      </c>
+      <c r="AE51">
+        <v>0</v>
+      </c>
+      <c r="AF51">
+        <v>0</v>
+      </c>
+      <c r="AG51">
+        <v>0</v>
+      </c>
+      <c r="AH51">
+        <v>0</v>
+      </c>
+      <c r="AI51">
+        <v>0</v>
+      </c>
+      <c r="AJ51">
+        <v>0</v>
+      </c>
+      <c r="AK51">
+        <v>0</v>
+      </c>
+      <c r="AL51">
+        <v>0</v>
+      </c>
+      <c r="AM51">
+        <v>0</v>
+      </c>
+      <c r="AN51">
+        <v>0</v>
+      </c>
+      <c r="AO51">
+        <v>0</v>
+      </c>
+      <c r="AP51">
+        <v>0</v>
+      </c>
+      <c r="AQ51">
+        <v>0</v>
+      </c>
+      <c r="AR51">
+        <v>0</v>
+      </c>
+      <c r="AS51">
+        <v>0</v>
+      </c>
+      <c r="AT51">
+        <v>0</v>
+      </c>
+      <c r="AU51">
+        <v>0</v>
+      </c>
+      <c r="AV51">
+        <v>0</v>
+      </c>
+      <c r="AW51">
+        <v>0</v>
+      </c>
+      <c r="AX51">
+        <v>0</v>
+      </c>
+      <c r="AY51">
+        <v>0</v>
+      </c>
+      <c r="AZ51">
+        <v>0</v>
+      </c>
+      <c r="BA51">
+        <v>0</v>
+      </c>
+      <c r="BB51">
+        <v>0</v>
+      </c>
+      <c r="BC51">
+        <v>0</v>
+      </c>
+      <c r="BD51">
+        <v>0</v>
+      </c>
+      <c r="BE51">
+        <v>0</v>
+      </c>
+      <c r="BF51">
+        <v>0</v>
+      </c>
+      <c r="BG51">
+        <v>0</v>
+      </c>
+      <c r="BH51">
+        <v>0</v>
+      </c>
+      <c r="BI51">
+        <v>0</v>
+      </c>
+      <c r="BJ51">
+        <v>0</v>
+      </c>
+      <c r="BK51">
+        <v>0</v>
+      </c>
+      <c r="BL51">
+        <v>0</v>
+      </c>
+      <c r="BM51">
+        <v>0</v>
+      </c>
+      <c r="BN51">
+        <v>0</v>
+      </c>
+      <c r="BO51">
+        <v>0</v>
+      </c>
+      <c r="BP51">
+        <v>0</v>
+      </c>
+      <c r="BQ51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:69">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:69">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:69">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:69">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:69">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:69">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:69">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:69">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:69">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:69">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:69">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:69">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:69">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:66">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:66">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:66">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:66">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:66">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:66">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:66">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:66">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:66">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:66">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:66">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:66">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C76">
-        <v>33.3333333</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>799.9999992</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>0</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>0</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>0</v>
+      </c>
+      <c r="X76">
+        <v>0</v>
+      </c>
+      <c r="Y76">
+        <v>0</v>
+      </c>
+      <c r="Z76">
+        <v>0</v>
+      </c>
+      <c r="AA76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:66">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:66">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:66">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="C79">
+        <v>33.3333333</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+      <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="U79">
+        <v>0</v>
+      </c>
+      <c r="V79">
+        <v>0</v>
+      </c>
+      <c r="W79">
+        <v>0</v>
+      </c>
+      <c r="X79">
+        <v>0</v>
+      </c>
+      <c r="Y79">
+        <v>0</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+      <c r="AA79">
+        <v>0</v>
+      </c>
+      <c r="AB79">
+        <v>0</v>
+      </c>
+      <c r="AC79">
+        <v>0</v>
+      </c>
+      <c r="AD79">
+        <v>0</v>
+      </c>
+      <c r="AE79">
+        <v>0</v>
+      </c>
+      <c r="AF79">
+        <v>0</v>
+      </c>
+      <c r="AG79">
+        <v>0</v>
+      </c>
+      <c r="AH79">
+        <v>0</v>
+      </c>
+      <c r="AI79">
+        <v>0</v>
+      </c>
+      <c r="AJ79">
+        <v>0</v>
+      </c>
+      <c r="AK79">
+        <v>0</v>
+      </c>
+      <c r="AL79">
+        <v>0</v>
+      </c>
+      <c r="AM79">
+        <v>0</v>
+      </c>
+      <c r="AN79">
+        <v>0</v>
+      </c>
+      <c r="AO79">
+        <v>0</v>
+      </c>
+      <c r="AP79">
+        <v>0</v>
+      </c>
+      <c r="AQ79">
+        <v>0</v>
+      </c>
+      <c r="AR79">
+        <v>0</v>
+      </c>
+      <c r="AS79">
+        <v>0</v>
+      </c>
+      <c r="AT79">
+        <v>0</v>
+      </c>
+      <c r="AU79">
+        <v>0</v>
+      </c>
+      <c r="AV79">
+        <v>0</v>
+      </c>
+      <c r="AW79">
+        <v>0</v>
+      </c>
+      <c r="AX79">
+        <v>0</v>
+      </c>
+      <c r="AY79">
+        <v>0</v>
+      </c>
+      <c r="AZ79">
+        <v>0</v>
+      </c>
+      <c r="BA79">
+        <v>0</v>
+      </c>
+      <c r="BB79">
+        <v>0</v>
+      </c>
+      <c r="BC79">
+        <v>0</v>
+      </c>
+      <c r="BD79">
+        <v>0</v>
+      </c>
+      <c r="BE79">
+        <v>0</v>
+      </c>
+      <c r="BF79">
+        <v>0</v>
+      </c>
+      <c r="BG79">
+        <v>0</v>
+      </c>
+      <c r="BH79">
+        <v>0</v>
+      </c>
+      <c r="BI79">
+        <v>0</v>
+      </c>
+      <c r="BJ79">
+        <v>0</v>
+      </c>
+      <c r="BK79">
+        <v>0</v>
+      </c>
+      <c r="BL79">
+        <v>0</v>
+      </c>
+      <c r="BM79">
+        <v>0</v>
+      </c>
+      <c r="BN79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:66">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:142">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:142">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:142">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:142">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:142">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:142">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:142">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:142">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:142">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:142">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:142">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:142">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:142">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:142">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:142">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:142">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C96">
-        <v>33.3333333</v>
+        <v>666.666666</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -1447,58 +2938,457 @@
       <c r="I96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
+      </c>
+      <c r="W96">
+        <v>0</v>
+      </c>
+      <c r="X96">
+        <v>0</v>
+      </c>
+      <c r="Y96">
+        <v>0</v>
+      </c>
+      <c r="Z96">
+        <v>0</v>
+      </c>
+      <c r="AA96">
+        <v>0</v>
+      </c>
+      <c r="AB96">
+        <v>0</v>
+      </c>
+      <c r="AC96">
+        <v>0</v>
+      </c>
+      <c r="AD96">
+        <v>0</v>
+      </c>
+      <c r="AE96">
+        <v>0</v>
+      </c>
+      <c r="AF96">
+        <v>0</v>
+      </c>
+      <c r="AG96">
+        <v>0</v>
+      </c>
+      <c r="AH96">
+        <v>0</v>
+      </c>
+      <c r="AI96">
+        <v>0</v>
+      </c>
+      <c r="AJ96">
+        <v>0</v>
+      </c>
+      <c r="AK96">
+        <v>0</v>
+      </c>
+      <c r="AL96">
+        <v>0</v>
+      </c>
+      <c r="AM96">
+        <v>0</v>
+      </c>
+      <c r="AN96">
+        <v>0</v>
+      </c>
+      <c r="AO96">
+        <v>0</v>
+      </c>
+      <c r="AP96">
+        <v>0</v>
+      </c>
+      <c r="AQ96">
+        <v>0</v>
+      </c>
+      <c r="AR96">
+        <v>0</v>
+      </c>
+      <c r="AS96">
+        <v>0</v>
+      </c>
+      <c r="AT96">
+        <v>0</v>
+      </c>
+      <c r="AU96">
+        <v>0</v>
+      </c>
+      <c r="AV96">
+        <v>0</v>
+      </c>
+      <c r="AW96">
+        <v>0</v>
+      </c>
+      <c r="AX96">
+        <v>0</v>
+      </c>
+      <c r="AY96">
+        <v>0</v>
+      </c>
+      <c r="AZ96">
+        <v>0</v>
+      </c>
+      <c r="BA96">
+        <v>0</v>
+      </c>
+      <c r="BB96">
+        <v>0</v>
+      </c>
+      <c r="BC96">
+        <v>0</v>
+      </c>
+      <c r="BD96">
+        <v>0</v>
+      </c>
+      <c r="BE96">
+        <v>0</v>
+      </c>
+      <c r="BF96">
+        <v>0</v>
+      </c>
+      <c r="BG96">
+        <v>0</v>
+      </c>
+      <c r="BH96">
+        <v>0</v>
+      </c>
+      <c r="BI96">
+        <v>0</v>
+      </c>
+      <c r="BJ96">
+        <v>0</v>
+      </c>
+      <c r="BK96">
+        <v>0</v>
+      </c>
+      <c r="BL96">
+        <v>0</v>
+      </c>
+      <c r="BM96">
+        <v>0</v>
+      </c>
+      <c r="BN96">
+        <v>0</v>
+      </c>
+      <c r="BO96">
+        <v>0</v>
+      </c>
+      <c r="BP96">
+        <v>0</v>
+      </c>
+      <c r="BQ96">
+        <v>0</v>
+      </c>
+      <c r="BR96">
+        <v>0</v>
+      </c>
+      <c r="BS96">
+        <v>0</v>
+      </c>
+      <c r="BT96">
+        <v>0</v>
+      </c>
+      <c r="BU96">
+        <v>0</v>
+      </c>
+      <c r="BV96">
+        <v>0</v>
+      </c>
+      <c r="BW96">
+        <v>0</v>
+      </c>
+      <c r="BX96">
+        <v>0</v>
+      </c>
+      <c r="BY96">
+        <v>0</v>
+      </c>
+      <c r="BZ96">
+        <v>0</v>
+      </c>
+      <c r="CA96">
+        <v>0</v>
+      </c>
+      <c r="CB96">
+        <v>0</v>
+      </c>
+      <c r="CC96">
+        <v>0</v>
+      </c>
+      <c r="CD96">
+        <v>0</v>
+      </c>
+      <c r="CE96">
+        <v>0</v>
+      </c>
+      <c r="CF96">
+        <v>0</v>
+      </c>
+      <c r="CG96">
+        <v>0</v>
+      </c>
+      <c r="CH96">
+        <v>0</v>
+      </c>
+      <c r="CI96">
+        <v>0</v>
+      </c>
+      <c r="CJ96">
+        <v>0</v>
+      </c>
+      <c r="CK96">
+        <v>0</v>
+      </c>
+      <c r="CL96">
+        <v>0</v>
+      </c>
+      <c r="CM96">
+        <v>0</v>
+      </c>
+      <c r="CN96">
+        <v>0</v>
+      </c>
+      <c r="CO96">
+        <v>0</v>
+      </c>
+      <c r="CP96">
+        <v>0</v>
+      </c>
+      <c r="CQ96">
+        <v>0</v>
+      </c>
+      <c r="CR96">
+        <v>0</v>
+      </c>
+      <c r="CS96">
+        <v>0</v>
+      </c>
+      <c r="CT96">
+        <v>0</v>
+      </c>
+      <c r="CU96">
+        <v>0</v>
+      </c>
+      <c r="CV96">
+        <v>0</v>
+      </c>
+      <c r="CW96">
+        <v>0</v>
+      </c>
+      <c r="CX96">
+        <v>0</v>
+      </c>
+      <c r="CY96">
+        <v>0</v>
+      </c>
+      <c r="CZ96">
+        <v>0</v>
+      </c>
+      <c r="DA96">
+        <v>0</v>
+      </c>
+      <c r="DB96">
+        <v>0</v>
+      </c>
+      <c r="DC96">
+        <v>0</v>
+      </c>
+      <c r="DD96">
+        <v>0</v>
+      </c>
+      <c r="DE96">
+        <v>0</v>
+      </c>
+      <c r="DF96">
+        <v>0</v>
+      </c>
+      <c r="DG96">
+        <v>0</v>
+      </c>
+      <c r="DH96">
+        <v>0</v>
+      </c>
+      <c r="DI96">
+        <v>0</v>
+      </c>
+      <c r="DJ96">
+        <v>0</v>
+      </c>
+      <c r="DK96">
+        <v>0</v>
+      </c>
+      <c r="DL96">
+        <v>0</v>
+      </c>
+      <c r="DM96">
+        <v>0</v>
+      </c>
+      <c r="DN96">
+        <v>0</v>
+      </c>
+      <c r="DO96">
+        <v>0</v>
+      </c>
+      <c r="DP96">
+        <v>0</v>
+      </c>
+      <c r="DQ96">
+        <v>0</v>
+      </c>
+      <c r="DR96">
+        <v>0</v>
+      </c>
+      <c r="DS96">
+        <v>0</v>
+      </c>
+      <c r="DT96">
+        <v>0</v>
+      </c>
+      <c r="DU96">
+        <v>0</v>
+      </c>
+      <c r="DV96">
+        <v>0</v>
+      </c>
+      <c r="DW96">
+        <v>0</v>
+      </c>
+      <c r="DX96">
+        <v>0</v>
+      </c>
+      <c r="DY96">
+        <v>0</v>
+      </c>
+      <c r="DZ96">
+        <v>0</v>
+      </c>
+      <c r="EA96">
+        <v>0</v>
+      </c>
+      <c r="EB96">
+        <v>0</v>
+      </c>
+      <c r="EC96">
+        <v>0</v>
+      </c>
+      <c r="ED96">
+        <v>0</v>
+      </c>
+      <c r="EE96">
+        <v>0</v>
+      </c>
+      <c r="EF96">
+        <v>0</v>
+      </c>
+      <c r="EG96">
+        <v>0</v>
+      </c>
+      <c r="EH96">
+        <v>0</v>
+      </c>
+      <c r="EI96">
+        <v>0</v>
+      </c>
+      <c r="EJ96">
+        <v>0</v>
+      </c>
+      <c r="EK96">
+        <v>0</v>
+      </c>
+      <c r="EL96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:145">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:145">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:145">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:145">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:145">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:145">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:145">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:145">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:145">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:145">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C106">
-        <v>33.3333333</v>
+        <v>666.666666</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -1518,73 +3408,481 @@
       <c r="I106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <v>0</v>
+      </c>
+      <c r="P106">
+        <v>0</v>
+      </c>
+      <c r="Q106">
+        <v>0</v>
+      </c>
+      <c r="R106">
+        <v>0</v>
+      </c>
+      <c r="S106">
+        <v>0</v>
+      </c>
+      <c r="T106">
+        <v>0</v>
+      </c>
+      <c r="U106">
+        <v>0</v>
+      </c>
+      <c r="V106">
+        <v>0</v>
+      </c>
+      <c r="W106">
+        <v>0</v>
+      </c>
+      <c r="X106">
+        <v>0</v>
+      </c>
+      <c r="Y106">
+        <v>0</v>
+      </c>
+      <c r="Z106">
+        <v>0</v>
+      </c>
+      <c r="AA106">
+        <v>0</v>
+      </c>
+      <c r="AB106">
+        <v>0</v>
+      </c>
+      <c r="AC106">
+        <v>0</v>
+      </c>
+      <c r="AD106">
+        <v>0</v>
+      </c>
+      <c r="AE106">
+        <v>0</v>
+      </c>
+      <c r="AF106">
+        <v>0</v>
+      </c>
+      <c r="AG106">
+        <v>0</v>
+      </c>
+      <c r="AH106">
+        <v>0</v>
+      </c>
+      <c r="AI106">
+        <v>0</v>
+      </c>
+      <c r="AJ106">
+        <v>0</v>
+      </c>
+      <c r="AK106">
+        <v>0</v>
+      </c>
+      <c r="AL106">
+        <v>0</v>
+      </c>
+      <c r="AM106">
+        <v>0</v>
+      </c>
+      <c r="AN106">
+        <v>0</v>
+      </c>
+      <c r="AO106">
+        <v>0</v>
+      </c>
+      <c r="AP106">
+        <v>0</v>
+      </c>
+      <c r="AQ106">
+        <v>0</v>
+      </c>
+      <c r="AR106">
+        <v>0</v>
+      </c>
+      <c r="AS106">
+        <v>0</v>
+      </c>
+      <c r="AT106">
+        <v>0</v>
+      </c>
+      <c r="AU106">
+        <v>0</v>
+      </c>
+      <c r="AV106">
+        <v>0</v>
+      </c>
+      <c r="AW106">
+        <v>0</v>
+      </c>
+      <c r="AX106">
+        <v>0</v>
+      </c>
+      <c r="AY106">
+        <v>0</v>
+      </c>
+      <c r="AZ106">
+        <v>0</v>
+      </c>
+      <c r="BA106">
+        <v>0</v>
+      </c>
+      <c r="BB106">
+        <v>0</v>
+      </c>
+      <c r="BC106">
+        <v>0</v>
+      </c>
+      <c r="BD106">
+        <v>0</v>
+      </c>
+      <c r="BE106">
+        <v>0</v>
+      </c>
+      <c r="BF106">
+        <v>0</v>
+      </c>
+      <c r="BG106">
+        <v>0</v>
+      </c>
+      <c r="BH106">
+        <v>0</v>
+      </c>
+      <c r="BI106">
+        <v>0</v>
+      </c>
+      <c r="BJ106">
+        <v>0</v>
+      </c>
+      <c r="BK106">
+        <v>0</v>
+      </c>
+      <c r="BL106">
+        <v>0</v>
+      </c>
+      <c r="BM106">
+        <v>0</v>
+      </c>
+      <c r="BN106">
+        <v>0</v>
+      </c>
+      <c r="BO106">
+        <v>0</v>
+      </c>
+      <c r="BP106">
+        <v>0</v>
+      </c>
+      <c r="BQ106">
+        <v>0</v>
+      </c>
+      <c r="BR106">
+        <v>0</v>
+      </c>
+      <c r="BS106">
+        <v>0</v>
+      </c>
+      <c r="BT106">
+        <v>0</v>
+      </c>
+      <c r="BU106">
+        <v>0</v>
+      </c>
+      <c r="BV106">
+        <v>0</v>
+      </c>
+      <c r="BW106">
+        <v>0</v>
+      </c>
+      <c r="BX106">
+        <v>0</v>
+      </c>
+      <c r="BY106">
+        <v>0</v>
+      </c>
+      <c r="BZ106">
+        <v>0</v>
+      </c>
+      <c r="CA106">
+        <v>0</v>
+      </c>
+      <c r="CB106">
+        <v>0</v>
+      </c>
+      <c r="CC106">
+        <v>0</v>
+      </c>
+      <c r="CD106">
+        <v>0</v>
+      </c>
+      <c r="CE106">
+        <v>0</v>
+      </c>
+      <c r="CF106">
+        <v>0</v>
+      </c>
+      <c r="CG106">
+        <v>0</v>
+      </c>
+      <c r="CH106">
+        <v>0</v>
+      </c>
+      <c r="CI106">
+        <v>0</v>
+      </c>
+      <c r="CJ106">
+        <v>0</v>
+      </c>
+      <c r="CK106">
+        <v>0</v>
+      </c>
+      <c r="CL106">
+        <v>0</v>
+      </c>
+      <c r="CM106">
+        <v>0</v>
+      </c>
+      <c r="CN106">
+        <v>0</v>
+      </c>
+      <c r="CO106">
+        <v>0</v>
+      </c>
+      <c r="CP106">
+        <v>0</v>
+      </c>
+      <c r="CQ106">
+        <v>0</v>
+      </c>
+      <c r="CR106">
+        <v>0</v>
+      </c>
+      <c r="CS106">
+        <v>0</v>
+      </c>
+      <c r="CT106">
+        <v>0</v>
+      </c>
+      <c r="CU106">
+        <v>0</v>
+      </c>
+      <c r="CV106">
+        <v>0</v>
+      </c>
+      <c r="CW106">
+        <v>0</v>
+      </c>
+      <c r="CX106">
+        <v>0</v>
+      </c>
+      <c r="CY106">
+        <v>0</v>
+      </c>
+      <c r="CZ106">
+        <v>0</v>
+      </c>
+      <c r="DA106">
+        <v>0</v>
+      </c>
+      <c r="DB106">
+        <v>0</v>
+      </c>
+      <c r="DC106">
+        <v>0</v>
+      </c>
+      <c r="DD106">
+        <v>0</v>
+      </c>
+      <c r="DE106">
+        <v>0</v>
+      </c>
+      <c r="DF106">
+        <v>0</v>
+      </c>
+      <c r="DG106">
+        <v>0</v>
+      </c>
+      <c r="DH106">
+        <v>0</v>
+      </c>
+      <c r="DI106">
+        <v>0</v>
+      </c>
+      <c r="DJ106">
+        <v>0</v>
+      </c>
+      <c r="DK106">
+        <v>0</v>
+      </c>
+      <c r="DL106">
+        <v>0</v>
+      </c>
+      <c r="DM106">
+        <v>0</v>
+      </c>
+      <c r="DN106">
+        <v>0</v>
+      </c>
+      <c r="DO106">
+        <v>0</v>
+      </c>
+      <c r="DP106">
+        <v>0</v>
+      </c>
+      <c r="DQ106">
+        <v>0</v>
+      </c>
+      <c r="DR106">
+        <v>0</v>
+      </c>
+      <c r="DS106">
+        <v>0</v>
+      </c>
+      <c r="DT106">
+        <v>0</v>
+      </c>
+      <c r="DU106">
+        <v>0</v>
+      </c>
+      <c r="DV106">
+        <v>0</v>
+      </c>
+      <c r="DW106">
+        <v>0</v>
+      </c>
+      <c r="DX106">
+        <v>0</v>
+      </c>
+      <c r="DY106">
+        <v>0</v>
+      </c>
+      <c r="DZ106">
+        <v>0</v>
+      </c>
+      <c r="EA106">
+        <v>0</v>
+      </c>
+      <c r="EB106">
+        <v>0</v>
+      </c>
+      <c r="EC106">
+        <v>0</v>
+      </c>
+      <c r="ED106">
+        <v>0</v>
+      </c>
+      <c r="EE106">
+        <v>0</v>
+      </c>
+      <c r="EF106">
+        <v>0</v>
+      </c>
+      <c r="EG106">
+        <v>0</v>
+      </c>
+      <c r="EH106">
+        <v>0</v>
+      </c>
+      <c r="EI106">
+        <v>0</v>
+      </c>
+      <c r="EJ106">
+        <v>0</v>
+      </c>
+      <c r="EK106">
+        <v>0</v>
+      </c>
+      <c r="EL106">
+        <v>0</v>
+      </c>
+      <c r="EM106">
+        <v>0</v>
+      </c>
+      <c r="EN106">
+        <v>0</v>
+      </c>
+      <c r="EO106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:145">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:145">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:145">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:145">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:145">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:145">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:81">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:81">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:81">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:81">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:81">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:81">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:81">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C119">
-        <v>33.3333333</v>
+        <v>833.3333325</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -1593,225 +3891,534 @@
         <v>0</v>
       </c>
       <c r="F119">
-        <v>33.3333333</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>0</v>
+      </c>
+      <c r="O119">
+        <v>0</v>
+      </c>
+      <c r="P119">
+        <v>0</v>
+      </c>
+      <c r="Q119">
+        <v>0</v>
+      </c>
+      <c r="R119">
+        <v>0</v>
+      </c>
+      <c r="S119">
+        <v>0</v>
+      </c>
+      <c r="T119">
+        <v>0</v>
+      </c>
+      <c r="U119">
+        <v>0</v>
+      </c>
+      <c r="V119">
+        <v>0</v>
+      </c>
+      <c r="W119">
+        <v>0</v>
+      </c>
+      <c r="X119">
+        <v>0</v>
+      </c>
+      <c r="Y119">
+        <v>0</v>
+      </c>
+      <c r="Z119">
+        <v>0</v>
+      </c>
+      <c r="AA119">
+        <v>0</v>
+      </c>
+      <c r="AB119">
+        <v>0</v>
+      </c>
+      <c r="AC119">
+        <v>0</v>
+      </c>
+      <c r="AD119">
+        <v>0</v>
+      </c>
+      <c r="AE119">
+        <v>0</v>
+      </c>
+      <c r="AF119">
+        <v>0</v>
+      </c>
+      <c r="AG119">
+        <v>0</v>
+      </c>
+      <c r="AH119">
+        <v>0</v>
+      </c>
+      <c r="AI119">
+        <v>0</v>
+      </c>
+      <c r="AJ119">
+        <v>0</v>
+      </c>
+      <c r="AK119">
+        <v>0</v>
+      </c>
+      <c r="AL119">
+        <v>0</v>
+      </c>
+      <c r="AM119">
+        <v>0</v>
+      </c>
+      <c r="AN119">
+        <v>0</v>
+      </c>
+      <c r="AO119">
+        <v>0</v>
+      </c>
+      <c r="AP119">
+        <v>0</v>
+      </c>
+      <c r="AQ119">
+        <v>0</v>
+      </c>
+      <c r="AR119">
+        <v>0</v>
+      </c>
+      <c r="AS119">
+        <v>0</v>
+      </c>
+      <c r="AT119">
+        <v>0</v>
+      </c>
+      <c r="AU119">
+        <v>0</v>
+      </c>
+      <c r="AV119">
+        <v>0</v>
+      </c>
+      <c r="AW119">
+        <v>0</v>
+      </c>
+      <c r="AX119">
+        <v>0</v>
+      </c>
+      <c r="AY119">
+        <v>0</v>
+      </c>
+      <c r="AZ119">
+        <v>0</v>
+      </c>
+      <c r="BA119">
+        <v>0</v>
+      </c>
+      <c r="BB119">
+        <v>0</v>
+      </c>
+      <c r="BC119">
+        <v>0</v>
+      </c>
+      <c r="BD119">
+        <v>0</v>
+      </c>
+      <c r="BE119">
+        <v>0</v>
+      </c>
+      <c r="BF119">
+        <v>0</v>
+      </c>
+      <c r="BG119">
+        <v>0</v>
+      </c>
+      <c r="BH119">
+        <v>0</v>
+      </c>
+      <c r="BI119">
+        <v>0</v>
+      </c>
+      <c r="BJ119">
+        <v>0</v>
+      </c>
+      <c r="BK119">
+        <v>0</v>
+      </c>
+      <c r="BL119">
+        <v>666.666666</v>
+      </c>
+      <c r="BM119">
+        <v>0</v>
+      </c>
+      <c r="BN119">
+        <v>0</v>
+      </c>
+      <c r="BO119">
+        <v>0</v>
+      </c>
+      <c r="BP119">
+        <v>0</v>
+      </c>
+      <c r="BQ119">
+        <v>0</v>
+      </c>
+      <c r="BR119">
+        <v>0</v>
+      </c>
+      <c r="BS119">
+        <v>0</v>
+      </c>
+      <c r="BT119">
+        <v>0</v>
+      </c>
+      <c r="BU119">
+        <v>0</v>
+      </c>
+      <c r="BV119">
+        <v>0</v>
+      </c>
+      <c r="BW119">
+        <v>0</v>
+      </c>
+      <c r="BX119">
+        <v>0</v>
+      </c>
+      <c r="BY119">
+        <v>0</v>
+      </c>
+      <c r="BZ119">
+        <v>0</v>
+      </c>
+      <c r="CA119">
+        <v>0</v>
+      </c>
+      <c r="CB119">
+        <v>0</v>
+      </c>
+      <c r="CC119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:81">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:81">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:81">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:81">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:81">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:81">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:81">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:81">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:81">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:4">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:4">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:4">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:4">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:4">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:4">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:4">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:4">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="C144">
+        <v>66.6666666</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:31">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C145">
-        <v>133.3333332</v>
+        <v>2133.3333312</v>
       </c>
       <c r="D145">
         <v>0</v>
       </c>
       <c r="E145">
-        <v>66.6666666</v>
+        <v>0</v>
       </c>
       <c r="F145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+        <v>1733.3333316</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+      <c r="M145">
+        <v>0</v>
+      </c>
+      <c r="N145">
+        <v>0</v>
+      </c>
+      <c r="O145">
+        <v>0</v>
+      </c>
+      <c r="P145">
+        <v>0</v>
+      </c>
+      <c r="Q145">
+        <v>0</v>
+      </c>
+      <c r="R145">
+        <v>0</v>
+      </c>
+      <c r="S145">
+        <v>0</v>
+      </c>
+      <c r="T145">
+        <v>0</v>
+      </c>
+      <c r="U145">
+        <v>0</v>
+      </c>
+      <c r="V145">
+        <v>0</v>
+      </c>
+      <c r="W145">
+        <v>0</v>
+      </c>
+      <c r="X145">
+        <v>0</v>
+      </c>
+      <c r="Y145">
+        <v>0</v>
+      </c>
+      <c r="Z145">
+        <v>0</v>
+      </c>
+      <c r="AA145">
+        <v>0</v>
+      </c>
+      <c r="AB145">
+        <v>0</v>
+      </c>
+      <c r="AC145">
+        <v>0</v>
+      </c>
+      <c r="AD145">
+        <v>0</v>
+      </c>
+      <c r="AE145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:31">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:31">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:31">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:31">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:31">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:31">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:31">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:31">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:31">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:31">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:31">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C156">
-        <v>133.3333332</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
+        <v>2233.3333311</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:31">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:31">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:31">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:31">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
fix: discard number in current frame if  len of numbers is smaller than previous numbers
</commit_message>
<xml_diff>
--- a/Resources/finaldata.xlsx
+++ b/Resources/finaldata.xlsx
@@ -1313,90 +1313,6 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>66.6666666</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:145">
       <c r="A3" s="1" t="s">
@@ -1435,117 +1351,6 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3">
-        <v>33.3333333</v>
-      </c>
-      <c r="O3">
-        <v>33.3333333</v>
-      </c>
-      <c r="P3">
-        <v>133.3333332</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="AU3">
-        <v>0</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AW3">
-        <v>0</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:145">
       <c r="A4" s="1" t="s">
@@ -1567,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>933.3333324</v>
+        <v>899.9999991</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1637,9 +1442,6 @@
       </c>
       <c r="Z7">
         <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>2033.3333313</v>
       </c>
     </row>
     <row r="8" spans="1:145">
@@ -1745,28 +1547,223 @@
       <c r="D14">
         <v>0</v>
       </c>
+      <c r="E14">
+        <v>33.3333333</v>
+      </c>
+      <c r="F14">
+        <v>2033.3333313</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
+        <v>0</v>
+      </c>
+      <c r="AS14">
+        <v>0</v>
+      </c>
+      <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>0</v>
+      </c>
+      <c r="AX14">
+        <v>0</v>
+      </c>
+      <c r="AY14">
+        <v>0</v>
+      </c>
+      <c r="AZ14">
+        <v>0</v>
+      </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>0</v>
+      </c>
+      <c r="BF14">
+        <v>0</v>
+      </c>
+      <c r="BG14">
+        <v>0</v>
+      </c>
+      <c r="BH14">
+        <v>0</v>
+      </c>
+      <c r="BI14">
+        <v>0</v>
+      </c>
+      <c r="BJ14">
+        <v>0</v>
+      </c>
+      <c r="BK14">
+        <v>0</v>
+      </c>
+      <c r="BL14">
+        <v>0</v>
+      </c>
+      <c r="BM14">
+        <v>0</v>
+      </c>
+      <c r="BN14">
+        <v>0</v>
+      </c>
+      <c r="BO14">
+        <v>0</v>
+      </c>
+      <c r="BP14">
+        <v>0</v>
+      </c>
+      <c r="BQ14">
+        <v>0</v>
+      </c>
+      <c r="BR14">
+        <v>0</v>
+      </c>
+      <c r="BS14">
+        <v>0</v>
+      </c>
+      <c r="BT14">
+        <v>33.3333333</v>
+      </c>
+      <c r="BU14">
+        <v>33.3333333</v>
+      </c>
+      <c r="BV14">
+        <v>133.3333332</v>
+      </c>
     </row>
     <row r="15" spans="1:145">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15">
-        <v>99.99999990000001</v>
-      </c>
-      <c r="D15">
-        <v>33.3333333</v>
-      </c>
-      <c r="E15">
-        <v>33.3333333</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
+        <v>66.6666666</v>
       </c>
     </row>
     <row r="16" spans="1:145">
@@ -1949,7 +1946,7 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>1166.6666655</v>
+        <v>1133.3333322</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2210,17 +2207,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:69">
+    <row r="49" spans="1:70">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:69">
+    <row r="50" spans="1:70">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:69">
+    <row r="51" spans="1:70">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2425,128 +2422,131 @@
       <c r="BQ51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:69">
+      <c r="BR51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:70">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:69">
+    <row r="53" spans="1:70">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:69">
+    <row r="54" spans="1:70">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:69">
+    <row r="55" spans="1:70">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:69">
+    <row r="56" spans="1:70">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:69">
+    <row r="57" spans="1:70">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:69">
+    <row r="58" spans="1:70">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:69">
+    <row r="59" spans="1:70">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:69">
+    <row r="60" spans="1:70">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:69">
+    <row r="61" spans="1:70">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:69">
+    <row r="62" spans="1:70">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:69">
+    <row r="63" spans="1:70">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:69">
+    <row r="64" spans="1:70">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:66">
+    <row r="65" spans="1:27">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:66">
+    <row r="66" spans="1:27">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:66">
+    <row r="67" spans="1:27">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:66">
+    <row r="68" spans="1:27">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:66">
+    <row r="69" spans="1:27">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:66">
+    <row r="70" spans="1:27">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:66">
+    <row r="71" spans="1:27">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:66">
+    <row r="72" spans="1:27">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:66">
+    <row r="73" spans="1:27">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:66">
+    <row r="74" spans="1:27">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:66">
+    <row r="75" spans="1:27">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:66">
+    <row r="76" spans="1:27">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -2626,214 +2626,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:66">
+    <row r="77" spans="1:27">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:66">
+    <row r="78" spans="1:27">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:66">
+    <row r="79" spans="1:27">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C79">
-        <v>33.3333333</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
-      <c r="M79">
-        <v>0</v>
-      </c>
-      <c r="N79">
-        <v>0</v>
-      </c>
-      <c r="O79">
-        <v>0</v>
-      </c>
-      <c r="P79">
-        <v>0</v>
-      </c>
-      <c r="Q79">
-        <v>0</v>
-      </c>
-      <c r="R79">
-        <v>0</v>
-      </c>
-      <c r="S79">
-        <v>0</v>
-      </c>
-      <c r="T79">
-        <v>0</v>
-      </c>
-      <c r="U79">
-        <v>0</v>
-      </c>
-      <c r="V79">
-        <v>0</v>
-      </c>
-      <c r="W79">
-        <v>0</v>
-      </c>
-      <c r="X79">
-        <v>0</v>
-      </c>
-      <c r="Y79">
-        <v>0</v>
-      </c>
-      <c r="Z79">
-        <v>0</v>
-      </c>
-      <c r="AA79">
-        <v>0</v>
-      </c>
-      <c r="AB79">
-        <v>0</v>
-      </c>
-      <c r="AC79">
-        <v>0</v>
-      </c>
-      <c r="AD79">
-        <v>0</v>
-      </c>
-      <c r="AE79">
-        <v>0</v>
-      </c>
-      <c r="AF79">
-        <v>0</v>
-      </c>
-      <c r="AG79">
-        <v>0</v>
-      </c>
-      <c r="AH79">
-        <v>0</v>
-      </c>
-      <c r="AI79">
-        <v>0</v>
-      </c>
-      <c r="AJ79">
-        <v>0</v>
-      </c>
-      <c r="AK79">
-        <v>0</v>
-      </c>
-      <c r="AL79">
-        <v>0</v>
-      </c>
-      <c r="AM79">
-        <v>0</v>
-      </c>
-      <c r="AN79">
-        <v>0</v>
-      </c>
-      <c r="AO79">
-        <v>0</v>
-      </c>
-      <c r="AP79">
-        <v>0</v>
-      </c>
-      <c r="AQ79">
-        <v>0</v>
-      </c>
-      <c r="AR79">
-        <v>0</v>
-      </c>
-      <c r="AS79">
-        <v>0</v>
-      </c>
-      <c r="AT79">
-        <v>0</v>
-      </c>
-      <c r="AU79">
-        <v>0</v>
-      </c>
-      <c r="AV79">
-        <v>0</v>
-      </c>
-      <c r="AW79">
-        <v>0</v>
-      </c>
-      <c r="AX79">
-        <v>0</v>
-      </c>
-      <c r="AY79">
-        <v>0</v>
-      </c>
-      <c r="AZ79">
-        <v>0</v>
-      </c>
-      <c r="BA79">
-        <v>0</v>
-      </c>
-      <c r="BB79">
-        <v>0</v>
-      </c>
-      <c r="BC79">
-        <v>0</v>
-      </c>
-      <c r="BD79">
-        <v>0</v>
-      </c>
-      <c r="BE79">
-        <v>0</v>
-      </c>
-      <c r="BF79">
-        <v>0</v>
-      </c>
-      <c r="BG79">
-        <v>0</v>
-      </c>
-      <c r="BH79">
-        <v>0</v>
-      </c>
-      <c r="BI79">
-        <v>0</v>
-      </c>
-      <c r="BJ79">
-        <v>0</v>
-      </c>
-      <c r="BK79">
-        <v>0</v>
-      </c>
-      <c r="BL79">
-        <v>0</v>
-      </c>
-      <c r="BM79">
-        <v>0</v>
-      </c>
-      <c r="BN79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:66">
+    </row>
+    <row r="80" spans="1:27">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -4164,82 +3972,82 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:36">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:36">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:36">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:36">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:36">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:36">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:36">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:36">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:36">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:36">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:36">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:36">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:36">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:36">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:36">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:36">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -4249,176 +4057,368 @@
       <c r="D144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:31">
+      <c r="E144">
+        <v>33.3333333</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144">
+        <v>0</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144">
+        <v>0</v>
+      </c>
+      <c r="O144">
+        <v>0</v>
+      </c>
+      <c r="P144">
+        <v>0</v>
+      </c>
+      <c r="Q144">
+        <v>0</v>
+      </c>
+      <c r="R144">
+        <v>0</v>
+      </c>
+      <c r="S144">
+        <v>0</v>
+      </c>
+      <c r="T144">
+        <v>0</v>
+      </c>
+      <c r="U144">
+        <v>0</v>
+      </c>
+      <c r="V144">
+        <v>0</v>
+      </c>
+      <c r="W144">
+        <v>0</v>
+      </c>
+      <c r="X144">
+        <v>0</v>
+      </c>
+      <c r="Y144">
+        <v>0</v>
+      </c>
+      <c r="Z144">
+        <v>0</v>
+      </c>
+      <c r="AA144">
+        <v>0</v>
+      </c>
+      <c r="AB144">
+        <v>0</v>
+      </c>
+      <c r="AC144">
+        <v>0</v>
+      </c>
+      <c r="AD144">
+        <v>0</v>
+      </c>
+      <c r="AE144">
+        <v>0</v>
+      </c>
+      <c r="AF144">
+        <v>33.3333333</v>
+      </c>
+      <c r="AG144">
+        <v>33.3333333</v>
+      </c>
+      <c r="AH144">
+        <v>0</v>
+      </c>
+      <c r="AI144">
+        <v>0</v>
+      </c>
+      <c r="AJ144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:64">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C145">
-        <v>2133.3333312</v>
+        <v>2199.9999978</v>
       </c>
       <c r="D145">
         <v>0</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>33.3333333</v>
       </c>
       <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
+      </c>
+      <c r="M145">
+        <v>0</v>
+      </c>
+      <c r="N145">
+        <v>0</v>
+      </c>
+      <c r="O145">
+        <v>0</v>
+      </c>
+      <c r="P145">
+        <v>0</v>
+      </c>
+      <c r="Q145">
+        <v>0</v>
+      </c>
+      <c r="R145">
+        <v>0</v>
+      </c>
+      <c r="S145">
+        <v>0</v>
+      </c>
+      <c r="T145">
+        <v>0</v>
+      </c>
+      <c r="U145">
+        <v>0</v>
+      </c>
+      <c r="V145">
+        <v>0</v>
+      </c>
+      <c r="W145">
+        <v>0</v>
+      </c>
+      <c r="X145">
+        <v>0</v>
+      </c>
+      <c r="Y145">
+        <v>0</v>
+      </c>
+      <c r="Z145">
+        <v>0</v>
+      </c>
+      <c r="AA145">
+        <v>0</v>
+      </c>
+      <c r="AB145">
+        <v>0</v>
+      </c>
+      <c r="AC145">
+        <v>0</v>
+      </c>
+      <c r="AD145">
+        <v>0</v>
+      </c>
+      <c r="AE145">
+        <v>0</v>
+      </c>
+      <c r="AF145">
+        <v>0</v>
+      </c>
+      <c r="AG145">
+        <v>0</v>
+      </c>
+      <c r="AH145">
+        <v>0</v>
+      </c>
+      <c r="AI145">
+        <v>0</v>
+      </c>
+      <c r="AJ145">
+        <v>0</v>
+      </c>
+      <c r="AK145">
+        <v>0</v>
+      </c>
+      <c r="AL145">
+        <v>0</v>
+      </c>
+      <c r="AM145">
         <v>1733.3333316</v>
       </c>
-      <c r="G145">
-        <v>0</v>
-      </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
-      <c r="I145">
-        <v>0</v>
-      </c>
-      <c r="J145">
-        <v>0</v>
-      </c>
-      <c r="K145">
-        <v>0</v>
-      </c>
-      <c r="L145">
-        <v>0</v>
-      </c>
-      <c r="M145">
-        <v>0</v>
-      </c>
-      <c r="N145">
-        <v>0</v>
-      </c>
-      <c r="O145">
-        <v>0</v>
-      </c>
-      <c r="P145">
-        <v>0</v>
-      </c>
-      <c r="Q145">
-        <v>0</v>
-      </c>
-      <c r="R145">
-        <v>0</v>
-      </c>
-      <c r="S145">
-        <v>0</v>
-      </c>
-      <c r="T145">
-        <v>0</v>
-      </c>
-      <c r="U145">
-        <v>0</v>
-      </c>
-      <c r="V145">
-        <v>0</v>
-      </c>
-      <c r="W145">
-        <v>0</v>
-      </c>
-      <c r="X145">
-        <v>0</v>
-      </c>
-      <c r="Y145">
-        <v>0</v>
-      </c>
-      <c r="Z145">
-        <v>0</v>
-      </c>
-      <c r="AA145">
-        <v>0</v>
-      </c>
-      <c r="AB145">
-        <v>0</v>
-      </c>
-      <c r="AC145">
-        <v>0</v>
-      </c>
-      <c r="AD145">
-        <v>0</v>
-      </c>
-      <c r="AE145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:31">
+      <c r="AN145">
+        <v>0</v>
+      </c>
+      <c r="AO145">
+        <v>0</v>
+      </c>
+      <c r="AP145">
+        <v>0</v>
+      </c>
+      <c r="AQ145">
+        <v>0</v>
+      </c>
+      <c r="AR145">
+        <v>0</v>
+      </c>
+      <c r="AS145">
+        <v>0</v>
+      </c>
+      <c r="AT145">
+        <v>0</v>
+      </c>
+      <c r="AU145">
+        <v>0</v>
+      </c>
+      <c r="AV145">
+        <v>0</v>
+      </c>
+      <c r="AW145">
+        <v>0</v>
+      </c>
+      <c r="AX145">
+        <v>0</v>
+      </c>
+      <c r="AY145">
+        <v>0</v>
+      </c>
+      <c r="AZ145">
+        <v>0</v>
+      </c>
+      <c r="BA145">
+        <v>0</v>
+      </c>
+      <c r="BB145">
+        <v>0</v>
+      </c>
+      <c r="BC145">
+        <v>0</v>
+      </c>
+      <c r="BD145">
+        <v>0</v>
+      </c>
+      <c r="BE145">
+        <v>0</v>
+      </c>
+      <c r="BF145">
+        <v>0</v>
+      </c>
+      <c r="BG145">
+        <v>0</v>
+      </c>
+      <c r="BH145">
+        <v>0</v>
+      </c>
+      <c r="BI145">
+        <v>0</v>
+      </c>
+      <c r="BJ145">
+        <v>0</v>
+      </c>
+      <c r="BK145">
+        <v>0</v>
+      </c>
+      <c r="BL145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:64">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:31">
+    <row r="147" spans="1:64">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:31">
+    <row r="148" spans="1:64">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:31">
+    <row r="149" spans="1:64">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:31">
+    <row r="150" spans="1:64">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:31">
+    <row r="151" spans="1:64">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:31">
+    <row r="152" spans="1:64">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:31">
+    <row r="153" spans="1:64">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:31">
+    <row r="154" spans="1:64">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:31">
+    <row r="155" spans="1:64">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:31">
+    <row r="156" spans="1:64">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C156">
-        <v>2233.3333311</v>
-      </c>
-      <c r="D156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:31">
+        <v>2266.6666644</v>
+      </c>
+    </row>
+    <row r="157" spans="1:64">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:31">
+    <row r="158" spans="1:64">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:31">
+    <row r="159" spans="1:64">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:31">
+    <row r="160" spans="1:64">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
feat: prepare for process various videos
</commit_message>
<xml_diff>
--- a/Resources/finaldata.xlsx
+++ b/Resources/finaldata.xlsx
@@ -869,13 +869,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D167"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -885,179 +885,206 @@
       <c r="D1" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12">
         <v>233.3333331</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12">
+        <v>233.3333331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14">
         <v>99.99999990000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14">
+        <v>99.99999990000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C22">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C24">
         <v>66.6666666</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <v>66.6666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1142,369 +1169,381 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C51">
         <v>233.3333331</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51">
+        <v>233.3333331</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C76">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C96">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:4">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:4">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:4">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:4">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:4">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:4">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:4">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:4">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C106">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:6">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:6">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:6">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:6">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:6">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:6">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:6">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -1514,48 +1553,54 @@
       <c r="D119">
         <v>33.3333333</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119">
+        <v>33.3333333</v>
+      </c>
+      <c r="F119">
+        <v>33.3333333</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:6">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:6">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:6">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:6">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:6">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:6">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:6">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:6">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -1640,7 +1685,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:6">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -1650,116 +1695,125 @@
       <c r="D145">
         <v>66.6666666</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145">
+        <v>166.6666665</v>
+      </c>
+      <c r="F145">
+        <v>66.6666666</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:6">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:6">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:6">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:6">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:6">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:6">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:6">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:6">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:6">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:6">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:6">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:6">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:6">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:6">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C161">
         <v>166.6666665</v>
       </c>
-    </row>
-    <row r="162" spans="1:3">
+      <c r="D161">
+        <v>166.6666665</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:4">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:4">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:4">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>

</xml_diff>